<commit_message>
add vat price to all files.
</commit_message>
<xml_diff>
--- a/after-big-bang-files/Lenovo/X280/comission Q3.xlsx
+++ b/after-big-bang-files/Lenovo/X280/comission Q3.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickvibild/repo/TellusAmazonPictures/after-big-bang-files/Lenovo/X280/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickvibild/Library/Containers/com.microsoft.Excel/Data/after-big-bang-files/Lenovo/X280/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E3A033B-6F3B-AF4C-91EF-73E6501A2429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80854E0C-AA28-8E42-814C-3B4D9BB8A522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13220" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{A9D9BB96-DDCC-544A-B02D-787B9D6ABD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>US</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>5% commission</t>
+  </si>
+  <si>
+    <t>List Price with Tax for Display</t>
+  </si>
+  <si>
+    <t>list_price_with_tax</t>
   </si>
 </sst>
 </file>
@@ -110,10 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,9 +139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +179,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -278,7 +285,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,7 +427,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -428,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2CB4FC-E085-244D-8536-48767F6ED5BD}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:GK49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -440,7 +447,7 @@
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -476,8 +483,11 @@
       <c r="F2" s="1">
         <v>168.88</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1896.11</v>
       </c>
@@ -493,8 +503,11 @@
       <c r="F3" s="1">
         <v>588.85</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>1193.3499999999999</v>
       </c>
@@ -504,8 +517,12 @@
         <v>1962.84</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK4" s="3">
+        <f>K4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>253.38</v>
       </c>
@@ -515,8 +532,12 @@
         <v>226.8</v>
       </c>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK5" s="3">
+        <f>K5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -524,8 +545,12 @@
         <v>284.98</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK6" s="3">
+        <f>K6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -533,8 +558,12 @@
         <v>1258.8399999999999</v>
       </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK7" s="3">
+        <f>K7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -542,8 +571,12 @@
         <v>373.71</v>
       </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK8" s="3">
+        <f>K8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -551,15 +584,23 @@
         <v>776.62</v>
       </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK9" s="3">
+        <f>K9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK10" s="3">
+        <f>K10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -578,8 +619,12 @@
       <c r="F11" s="1">
         <v>657.86</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK11" s="3">
+        <f>K11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>1805.69</v>
       </c>
@@ -593,8 +638,12 @@
       <c r="F12" s="1">
         <v>253.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK12" s="3">
+        <f>K12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>2063.42</v>
       </c>
@@ -608,8 +657,12 @@
       <c r="F13" s="1">
         <v>219.36</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK13" s="3">
+        <f>K13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>303.05</v>
       </c>
@@ -619,8 +672,12 @@
         <v>627.66999999999996</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK14" s="3">
+        <f>K14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>1128.9000000000001</v>
       </c>
@@ -630,8 +687,12 @@
         <v>1450.69</v>
       </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK15" s="3">
+        <f>K15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>181.68</v>
       </c>
@@ -641,8 +702,12 @@
         <v>767.58</v>
       </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK16" s="3">
+        <f>K16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -650,8 +715,12 @@
         <v>776.36</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK17" s="3">
+        <f>K17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -659,8 +728,12 @@
         <v>345.32</v>
       </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK18" s="3">
+        <f>K18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -668,8 +741,12 @@
         <v>1961.5</v>
       </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK19" s="3">
+        <f>K19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -677,8 +754,12 @@
         <v>396.16</v>
       </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK20" s="3">
+        <f>K20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -686,8 +767,12 @@
         <v>569</v>
       </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK21" s="3">
+        <f>K21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -695,15 +780,23 @@
         <v>341.45</v>
       </c>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK22" s="3">
+        <f>K22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK23" s="3">
+        <f>K23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -722,8 +815,12 @@
       <c r="F24" s="1">
         <v>343.75</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK24" s="3">
+        <f>K24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>2053.9</v>
       </c>
@@ -739,8 +836,12 @@
       <c r="F25" s="1">
         <v>278</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK25" s="3">
+        <f>K25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>1765.62</v>
       </c>
@@ -750,8 +851,12 @@
         <v>551.78</v>
       </c>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK26" s="3">
+        <f>K26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>124.28</v>
       </c>
@@ -761,8 +866,12 @@
         <v>754.28</v>
       </c>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK27" s="3">
+        <f>K27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -770,8 +879,12 @@
         <v>831.84</v>
       </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK28" s="3">
+        <f>K28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -779,8 +892,12 @@
         <v>1110.68</v>
       </c>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK29" s="3">
+        <f>K29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -788,8 +905,12 @@
         <v>2067.58</v>
       </c>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK30" s="3">
+        <f>K30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -797,15 +918,23 @@
         <v>835.01</v>
       </c>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="GK31" s="3">
+        <f>K31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK32" s="3">
+        <f>K32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -829,8 +958,18 @@
         <f t="shared" si="0"/>
         <v>2510.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK33" s="3">
+        <f>K33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:193" x14ac:dyDescent="0.2">
+      <c r="GK34" s="3">
+        <f>K34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -855,8 +994,12 @@
       <c r="J35" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK35" s="3">
+        <f>K35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:193" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -888,76 +1031,138 @@
         <f>H36*0.05</f>
         <v>15280.884274999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK36" s="3">
+        <f>K36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK37" s="3">
+        <f>K37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK38" s="3">
+        <f>K38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK39" s="3">
+        <f>K39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK40" s="3">
+        <f>K40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK41" s="3">
+        <f>K41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK42" s="3">
+        <f>K42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK43" s="3">
+        <f>K43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK44" s="3">
+        <f>K44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="GK45" s="3">
+        <f>K45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:193" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
+      <c r="GK46" s="3">
+        <f>K46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:193" x14ac:dyDescent="0.2">
+      <c r="GK47" s="3">
+        <f>K47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:193" x14ac:dyDescent="0.2">
+      <c r="GK48" s="3">
+        <f>K48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="193:193" x14ac:dyDescent="0.2">
+      <c r="GK49" s="3">
+        <f>K49</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>